<commit_message>
Mar 2, 2025, 3:38 AM
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hosei\Desktop\Docs\Codes\Peng_Robinson_eos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{99E371C3-88CA-4D56-9B1A-BF764DE44865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83496CCA-CB98-41BD-8F8B-47B04A28452A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{B46AD3A4-F02F-4EF3-998F-7FA77B38839D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{B46AD3A4-F02F-4EF3-998F-7FA77B38839D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
   <si>
     <t>Temp</t>
   </si>
@@ -107,6 +108,21 @@
   </si>
   <si>
     <t>d (CO2)</t>
+  </si>
+  <si>
+    <t>Mw drug</t>
+  </si>
+  <si>
+    <t>Mw co2</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>rho</t>
+  </si>
+  <si>
+    <t>y1</t>
   </si>
 </sst>
 </file>
@@ -852,7 +868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD253055-DC9A-4168-A0E6-95A2E28FDC41}">
   <dimension ref="A1:Y639"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -9257,4 +9273,142 @@
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07DBD74B-6DB6-41EA-A387-9E1A3F2FF5EE}">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="B2">
+        <v>769</v>
+      </c>
+      <c r="C2">
+        <f>(A2*44.01)/((B2*598.5) + (A2*44.01))</f>
+        <v>2.0080720746810844E-6</v>
+      </c>
+      <c r="D2">
+        <f>C2*1000000</f>
+        <v>2.0080720746810843</v>
+      </c>
+      <c r="H2">
+        <v>598.5</v>
+      </c>
+      <c r="I2">
+        <v>44.01</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="B3">
+        <v>817</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C7" si="0">(A3*44.01)/((B3*598.5) + (A3*44.01))</f>
+        <v>2.3401165547451471E-6</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D7" si="1">C3*1000000</f>
+        <v>2.3401165547451472</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="B4">
+        <v>849</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>2.5117501139547866E-6</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>2.5117501139547866</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3.9E-2</v>
+      </c>
+      <c r="B5">
+        <v>875</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>3.277497313830071E-6</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>3.2774973138300711</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="B6">
+        <v>896</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>3.7751602916125805E-6</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>3.7751602916125804</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="B7">
+        <v>914</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>5.3098548279471017E-6</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>5.3098548279471016</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Mar 7, 2025, 4:15 AM
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hosei\Desktop\Docs\Codes\Peng_Robinson_eos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32228AFE-4B64-4968-97F1-2C18C31217DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600A5340-B38B-4650-B07F-97FE0A3C6B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B46AD3A4-F02F-4EF3-998F-7FA77B38839D}"/>
   </bookViews>
@@ -1256,7 +1256,7 @@
         <v>43</v>
       </c>
       <c r="B16" s="27">
-        <v>0.41070000000000001</v>
+        <v>0.89890000000000003</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -1273,7 +1273,7 @@
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="21">
         <f>B12*(B16^3) + B13*(B16^2) + B14*B16 + B15</f>
-        <v>-2.159534980714084E-5</v>
+        <v>0.4646328277722741</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1322,7 +1322,10 @@
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
+      <c r="D20" s="21">
+        <f>B12*B17^3 + B13*B17^2 + B14*B17 + B15</f>
+        <v>-0.1985779004250896</v>
+      </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>

</xml_diff>